<commit_message>
Add clustering and heatmap files
</commit_message>
<xml_diff>
--- a/example/Topic/60/LG/6040i10-2/1/k15/c10d5/H1H2.xlsx
+++ b/example/Topic/60/LG/6040i10-2/1/k15/c10d5/H1H2.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EDU\files\2013\example\Topic\60\LG\6040i10-2\1\k15\c10d5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{708B6FE3-3831-4B4C-B663-26BDE7C75B35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D514310A-8A30-4497-9499-F9688C2732D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1H2" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="2" r:id="rId2"/>
     <sheet name="3" sheetId="3" r:id="rId3"/>
     <sheet name="4" sheetId="4" r:id="rId4"/>
+    <sheet name="Kmeans-2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="8">
   <si>
     <t>l</t>
   </si>
@@ -36,11 +37,23 @@
   <si>
     <t>Cluster</t>
   </si>
+  <si>
+    <t>TP:</t>
+  </si>
+  <si>
+    <t>TN:</t>
+  </si>
+  <si>
+    <t>FP:</t>
+  </si>
+  <si>
+    <t>FN:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,9 +531,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -875,11 +889,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4240,11 +4254,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4252,7 +4266,7 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4260,7 +4274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4312,8 +4326,14 @@
       <c r="Q2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4365,8 +4385,14 @@
       <c r="Q3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4418,8 +4444,14 @@
       <c r="Q4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4471,8 +4503,14 @@
       <c r="Q5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4525,7 +4563,7 @@
         <v>3.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4578,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4631,7 +4669,7 @@
         <v>3.2399999999999998E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4684,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -4737,7 +4775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -4790,7 +4828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -4843,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4896,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4949,7 +4987,7 @@
         <v>9.1699999999999993E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -5002,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -7813,11 +7851,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11394,7 +11433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14968,4 +15007,587 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BC0D9E-5121-487E-B7C6-1256FD31171E}">
+  <dimension ref="A1:F68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add clustering and heatmap new files
</commit_message>
<xml_diff>
--- a/example/Topic/60/LG/6040i10-2/1/k15/c10d5/H1H2.xlsx
+++ b/example/Topic/60/LG/6040i10-2/1/k15/c10d5/H1H2.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EDU\files\2013\example\Topic\60\LG\6040i10-2\1\k15\c10d5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D514310A-8A30-4497-9499-F9688C2732D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5752E0D-C93B-4ACE-AB0E-56CBB48ADBCD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1H2" sheetId="1" r:id="rId1"/>
-    <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="Spectral-2" sheetId="2" r:id="rId2"/>
     <sheet name="3" sheetId="3" r:id="rId3"/>
     <sheet name="4" sheetId="4" r:id="rId4"/>
     <sheet name="Kmeans-2" sheetId="5" r:id="rId5"/>
@@ -15014,7 +15014,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>